<commit_message>
update NSAIDs drug resource mapping
</commit_message>
<xml_diff>
--- a/NSAID/Celecoxib_Drug_Resource_Mappings.xlsx
+++ b/NSAID/Celecoxib_Drug_Resource_Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\CYP2C9_NSAIDS\Implementation tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgong/Documents/Li thinkpad/CPIC/celecoxib/final/Implementation tables/Implementation tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F0D358-2786-4602-AAD6-4FD73EF9C85F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46B13FF-72E2-BF48-84FE-D7B498AB60C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Celecoxib" sheetId="25" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Drug or Ingredient</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>DB00482</t>
-  </si>
-  <si>
-    <t>C0538927</t>
   </si>
 </sst>
 </file>
@@ -616,19 +613,19 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="10.85546875" style="1"/>
+    <col min="4" max="4" width="13.1640625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -642,7 +639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -652,11 +649,11 @@
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
+      <c r="D2" s="8">
+        <v>140587</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -670,7 +667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -684,7 +681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -698,7 +695,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
     </row>
   </sheetData>

</xml_diff>